<commit_message>
Completion of Utility PV example
Correction and completion of Utility PV Example.
</commit_message>
<xml_diff>
--- a/src/technology/utility-pv/utility-pv.xlsx
+++ b/src/technology/utility-pv/utility-pv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\utility-pv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/tghosh_nrel_gov/Documents/work_NREL/tyche/src/technology/utility-pv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{091439C3-444C-4131-A93A-CE653FCCFD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F044E88C-2B49-3746-9646-5F69E356B378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78D4C623-3986-C54F-BB36-B9C749FB82E4}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="2505" windowWidth="20910" windowHeight="11775" xr2:uid="{A613468B-4246-47D0-8059-797BD75C3238}"/>
+    <workbookView xWindow="43420" yWindow="-9900" windowWidth="21460" windowHeight="16780" activeTab="4" xr2:uid="{A613468B-4246-47D0-8059-797BD75C3238}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="100">
   <si>
     <t>Technology</t>
   </si>
@@ -333,6 +333,15 @@
   </si>
   <si>
     <t>Fast Progress on PV</t>
+  </si>
+  <si>
+    <t>Low R&amp;D Spending</t>
+  </si>
+  <si>
+    <t>Medium R&amp;D Spending</t>
+  </si>
+  <si>
+    <t>High R&amp;D Spending</t>
   </si>
 </sst>
 </file>
@@ -388,7 +397,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -676,7 +685,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -684,13 +693,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404BF247-5429-4E4B-9678-6277797CABB5}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,7 +729,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -733,7 +749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -756,7 +772,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -776,7 +792,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -799,7 +815,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -822,7 +838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -842,7 +858,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -862,6 +878,462 @@
         <v>27</v>
       </c>
       <c r="G8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>5.5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10">
+        <v>0.152</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>0.05</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>5.5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>0.152</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21">
+        <v>0.05</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23">
+        <v>5.5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <v>0.152</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28">
+        <v>0.05</v>
+      </c>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" t="s">
         <v>28</v>
       </c>
     </row>
@@ -874,13 +1346,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEB1B46-74EC-4182-94AB-66630EC1D78A}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="161" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +1378,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -938,11 +1410,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5423B8-8C49-451E-B763-E5AF0240ECDF}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="164" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -962,7 +1439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -982,7 +1459,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -999,7 +1476,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1016,7 +1493,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1033,7 +1510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1057,13 +1534,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09184F9C-6CBE-4249-A108-F70A85144612}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="143" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -1077,7 +1561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1086,6 +1570,39 @@
       </c>
       <c r="C2" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1095,13 +1612,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD7A7F6-C51A-4296-993F-ABD3322B9938}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1147,7 +1671,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1170,7 +1694,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1193,7 +1717,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1216,7 +1740,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1239,7 +1763,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1262,7 +1786,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1285,7 +1809,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1308,7 +1832,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1331,7 +1855,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1354,7 +1878,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1377,7 +1901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1400,7 +1924,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1423,7 +1947,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1443,6 +1967,972 @@
         <v>85</v>
       </c>
       <c r="G15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>243</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>180</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>2.33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>0.45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>9.4330000000000004E-3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>1.5512999999999999</v>
+      </c>
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <v>1000</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25">
+        <v>9</v>
+      </c>
+      <c r="E25">
+        <v>1000</v>
+      </c>
+      <c r="F25" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>0.27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>0.95</v>
+      </c>
+      <c r="F27" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28">
+        <v>0.9</v>
+      </c>
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29">
+        <v>13</v>
+      </c>
+      <c r="E29">
+        <v>400</v>
+      </c>
+      <c r="F29" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>72</v>
+      </c>
+      <c r="F30" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>243</v>
+      </c>
+      <c r="F31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32">
+        <v>180</v>
+      </c>
+      <c r="F32" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <v>2.33</v>
+      </c>
+      <c r="F33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>26</v>
+      </c>
+      <c r="F34" t="s">
+        <v>67</v>
+      </c>
+      <c r="G34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>0.45</v>
+      </c>
+      <c r="F35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+      <c r="E36">
+        <v>9.4330000000000004E-3</v>
+      </c>
+      <c r="F36" t="s">
+        <v>72</v>
+      </c>
+      <c r="G36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37">
+        <v>7</v>
+      </c>
+      <c r="E37">
+        <v>1.5512999999999999</v>
+      </c>
+      <c r="F37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38">
+        <v>8</v>
+      </c>
+      <c r="E38">
+        <v>1000</v>
+      </c>
+      <c r="F38" t="s">
+        <v>77</v>
+      </c>
+      <c r="G38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+      <c r="D39">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>1000</v>
+      </c>
+      <c r="F39" t="s">
+        <v>77</v>
+      </c>
+      <c r="G39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="E40">
+        <v>0.27</v>
+      </c>
+      <c r="F40" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41">
+        <v>11</v>
+      </c>
+      <c r="E41">
+        <v>0.95</v>
+      </c>
+      <c r="F41" t="s">
+        <v>70</v>
+      </c>
+      <c r="G41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42">
+        <v>12</v>
+      </c>
+      <c r="E42">
+        <v>0.9</v>
+      </c>
+      <c r="F42" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43">
+        <v>13</v>
+      </c>
+      <c r="E43">
+        <v>400</v>
+      </c>
+      <c r="F43" t="s">
+        <v>85</v>
+      </c>
+      <c r="G43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>72</v>
+      </c>
+      <c r="F44" t="s">
+        <v>59</v>
+      </c>
+      <c r="G44" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>243</v>
+      </c>
+      <c r="F45" t="s">
+        <v>61</v>
+      </c>
+      <c r="G45" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>180</v>
+      </c>
+      <c r="F46" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>2.33</v>
+      </c>
+      <c r="F47" t="s">
+        <v>65</v>
+      </c>
+      <c r="G47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>26</v>
+      </c>
+      <c r="F48" t="s">
+        <v>67</v>
+      </c>
+      <c r="G48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49">
+        <v>0.45</v>
+      </c>
+      <c r="F49" t="s">
+        <v>70</v>
+      </c>
+      <c r="G49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50">
+        <v>6</v>
+      </c>
+      <c r="E50">
+        <v>9.4330000000000004E-3</v>
+      </c>
+      <c r="F50" t="s">
+        <v>72</v>
+      </c>
+      <c r="G50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>96</v>
+      </c>
+      <c r="C51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51">
+        <v>7</v>
+      </c>
+      <c r="E51">
+        <v>1.5512999999999999</v>
+      </c>
+      <c r="F51" t="s">
+        <v>75</v>
+      </c>
+      <c r="G51" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="E52">
+        <v>1000</v>
+      </c>
+      <c r="F52" t="s">
+        <v>77</v>
+      </c>
+      <c r="G52" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" t="s">
+        <v>79</v>
+      </c>
+      <c r="D53">
+        <v>9</v>
+      </c>
+      <c r="E53">
+        <v>1000</v>
+      </c>
+      <c r="F53" t="s">
+        <v>77</v>
+      </c>
+      <c r="G53" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54">
+        <v>10</v>
+      </c>
+      <c r="E54">
+        <v>0.27</v>
+      </c>
+      <c r="F54" t="s">
+        <v>70</v>
+      </c>
+      <c r="G54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55">
+        <v>11</v>
+      </c>
+      <c r="E55">
+        <v>0.95</v>
+      </c>
+      <c r="F55" t="s">
+        <v>70</v>
+      </c>
+      <c r="G55" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>96</v>
+      </c>
+      <c r="C56" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56">
+        <v>12</v>
+      </c>
+      <c r="E56">
+        <v>0.9</v>
+      </c>
+      <c r="F56" t="s">
+        <v>70</v>
+      </c>
+      <c r="G56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" t="s">
+        <v>84</v>
+      </c>
+      <c r="D57">
+        <v>13</v>
+      </c>
+      <c r="E57">
+        <v>400</v>
+      </c>
+      <c r="F57" t="s">
+        <v>85</v>
+      </c>
+      <c r="G57" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1455,11 +2945,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582C6D20-8276-4D8D-A540-E889EFB05E57}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="161" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1476,7 +2966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1490,7 +2980,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1504,7 +2994,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1518,7 +3008,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1541,11 +3031,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B0404B-9994-498F-B4BE-63E960C20C4D}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="185" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1562,7 +3058,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1576,7 +3072,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1590,7 +3086,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1604,7 +3100,7 @@
         <v>4500000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
#144 updates utility pv to remove scenarios
</commit_message>
<xml_diff>
--- a/src/technology/utility-pv/utility-pv.xlsx
+++ b/src/technology/utility-pv/utility-pv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/tghosh_nrel_gov/Documents/work_NREL/tyche/src/technology/utility-pv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhanes\GitHub\tyche\src\technology\utility-pv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F044E88C-2B49-3746-9646-5F69E356B378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{78D4C623-3986-C54F-BB36-B9C749FB82E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC7A01D-3E64-4F26-BD12-0646E03E7CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43420" yWindow="-9900" windowWidth="21460" windowHeight="16780" activeTab="4" xr2:uid="{A613468B-4246-47D0-8059-797BD75C3238}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="6" xr2:uid="{A613468B-4246-47D0-8059-797BD75C3238}"/>
   </bookViews>
   <sheets>
     <sheet name="designs" sheetId="1" r:id="rId1"/>
@@ -42,14 +42,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="95">
   <si>
     <t>Technology</t>
   </si>
   <si>
-    <t>Scenario</t>
-  </si>
-  <si>
     <t>Variable</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>PV R&amp;D</t>
   </si>
   <si>
-    <t>No PV R&amp;D</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -317,19 +311,10 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Low PV R&amp;D</t>
-  </si>
-  <si>
     <t>Slow Progress on PV</t>
   </si>
   <si>
-    <t>Medium PV R&amp;D</t>
-  </si>
-  <si>
     <t>Moderate Progress on PV</t>
-  </si>
-  <si>
-    <t>High PV R&amp;D</t>
   </si>
   <si>
     <t>Fast Progress on PV</t>
@@ -397,7 +382,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -685,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -695,72 +680,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404BF247-5429-4E4B-9678-6277797CABB5}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
       </c>
       <c r="E2">
         <v>5.5</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
       <c r="E3">
         <v>0.152</v>
@@ -769,41 +754,41 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -812,107 +797,107 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
       </c>
       <c r="E6">
         <v>20</v>
       </c>
       <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>0.05</v>
       </c>
       <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>5.5</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10">
         <v>0.152</v>
@@ -921,41 +906,41 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -964,107 +949,107 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>22</v>
       </c>
       <c r="E13">
         <v>20</v>
       </c>
       <c r="F13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
         <v>23</v>
       </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14">
         <v>0.05</v>
       </c>
       <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" t="s">
         <v>27</v>
       </c>
-      <c r="G15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16">
         <v>5.5</v>
       </c>
       <c r="F16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>0.152</v>
@@ -1073,41 +1058,41 @@
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1116,107 +1101,107 @@
         <v>1</v>
       </c>
       <c r="G19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>94</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>22</v>
       </c>
       <c r="E20">
         <v>20</v>
       </c>
       <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
         <v>23</v>
       </c>
-      <c r="G20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21">
         <v>0.05</v>
       </c>
       <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
         <v>25</v>
       </c>
-      <c r="G21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" t="s">
         <v>27</v>
       </c>
-      <c r="G22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E23">
         <v>5.5</v>
       </c>
       <c r="F23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24">
         <v>0.152</v>
@@ -1225,41 +1210,41 @@
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
       <c r="F25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>96</v>
-      </c>
-      <c r="C26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" t="s">
-        <v>20</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1268,73 +1253,73 @@
         <v>1</v>
       </c>
       <c r="G26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>96</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>22</v>
       </c>
       <c r="E27">
         <v>20</v>
       </c>
       <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
         <v>23</v>
       </c>
-      <c r="G27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28">
         <v>0.05</v>
       </c>
       <c r="F28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" t="s">
         <v>25</v>
       </c>
-      <c r="G28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E29">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29" t="s">
         <v>27</v>
-      </c>
-      <c r="G29" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1346,59 +1331,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEB1B46-74EC-4182-94AB-66630EC1D78A}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScale="161" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>38</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>39</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1410,121 +1395,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC5423B8-8C49-451E-B763-E5AF0240ECDF}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="164" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
       <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1536,73 +1521,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09184F9C-6CBE-4249-A108-F70A85144612}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="143" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>52</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>54</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
       <c r="C2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1614,49 +1599,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD7A7F6-C51A-4296-993F-ABD3322B9938}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1665,21 +1650,21 @@
         <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1688,21 +1673,21 @@
         <v>243</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1711,21 +1696,21 @@
         <v>180</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1734,21 +1719,21 @@
         <v>2.33</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1757,21 +1742,21 @@
         <v>26</v>
       </c>
       <c r="F6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>67</v>
-      </c>
-      <c r="G6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -1780,21 +1765,21 @@
         <v>0.45</v>
       </c>
       <c r="F7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1803,21 +1788,21 @@
         <v>9.4330000000000004E-3</v>
       </c>
       <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>72</v>
-      </c>
-      <c r="G8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>74</v>
       </c>
       <c r="D9">
         <v>7</v>
@@ -1826,21 +1811,21 @@
         <v>1.5512999999999999</v>
       </c>
       <c r="F9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -1849,21 +1834,21 @@
         <v>1000</v>
       </c>
       <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
         <v>77</v>
-      </c>
-      <c r="G10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>79</v>
       </c>
       <c r="D11">
         <v>9</v>
@@ -1872,21 +1857,21 @@
         <v>1000</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>80</v>
       </c>
       <c r="D12">
         <v>10</v>
@@ -1895,21 +1880,21 @@
         <v>0.27</v>
       </c>
       <c r="F12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13">
         <v>11</v>
@@ -1918,21 +1903,21 @@
         <v>0.95</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D14">
         <v>12</v>
@@ -1941,21 +1926,21 @@
         <v>0.9</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D15">
         <v>13</v>
@@ -1964,21 +1949,21 @@
         <v>400</v>
       </c>
       <c r="F15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1987,21 +1972,21 @@
         <v>72</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2010,21 +1995,21 @@
         <v>243</v>
       </c>
       <c r="F17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -2033,21 +2018,21 @@
         <v>180</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -2056,21 +2041,21 @@
         <v>2.33</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -2079,21 +2064,21 @@
         <v>26</v>
       </c>
       <c r="F20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
         <v>67</v>
-      </c>
-      <c r="G20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" t="s">
-        <v>69</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -2102,21 +2087,21 @@
         <v>0.45</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D22">
         <v>6</v>
@@ -2125,21 +2110,21 @@
         <v>9.4330000000000004E-3</v>
       </c>
       <c r="F22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
         <v>72</v>
-      </c>
-      <c r="G22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" t="s">
-        <v>92</v>
-      </c>
-      <c r="C23" t="s">
-        <v>74</v>
       </c>
       <c r="D23">
         <v>7</v>
@@ -2148,21 +2133,21 @@
         <v>1.5512999999999999</v>
       </c>
       <c r="F23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D24">
         <v>8</v>
@@ -2171,21 +2156,21 @@
         <v>1000</v>
       </c>
       <c r="F24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
         <v>77</v>
-      </c>
-      <c r="G24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
       </c>
       <c r="D25">
         <v>9</v>
@@ -2194,21 +2179,21 @@
         <v>1000</v>
       </c>
       <c r="F25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" t="s">
-        <v>92</v>
-      </c>
-      <c r="C26" t="s">
-        <v>80</v>
       </c>
       <c r="D26">
         <v>10</v>
@@ -2217,21 +2202,21 @@
         <v>0.27</v>
       </c>
       <c r="F26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D27">
         <v>11</v>
@@ -2240,21 +2225,21 @@
         <v>0.95</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D28">
         <v>12</v>
@@ -2263,21 +2248,21 @@
         <v>0.9</v>
       </c>
       <c r="F28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D29">
         <v>13</v>
@@ -2286,21 +2271,21 @@
         <v>400</v>
       </c>
       <c r="F29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -2309,21 +2294,21 @@
         <v>72</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G30" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -2332,21 +2317,21 @@
         <v>243</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G31" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -2355,21 +2340,21 @@
         <v>180</v>
       </c>
       <c r="F32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -2378,21 +2363,21 @@
         <v>2.33</v>
       </c>
       <c r="F33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G33" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -2401,21 +2386,21 @@
         <v>26</v>
       </c>
       <c r="F34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" t="s">
         <v>67</v>
-      </c>
-      <c r="G34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" t="s">
-        <v>69</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -2424,21 +2409,21 @@
         <v>0.45</v>
       </c>
       <c r="F35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D36">
         <v>6</v>
@@ -2447,21 +2432,21 @@
         <v>9.4330000000000004E-3</v>
       </c>
       <c r="F36" t="s">
+        <v>70</v>
+      </c>
+      <c r="G36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
         <v>72</v>
-      </c>
-      <c r="G36" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" t="s">
-        <v>74</v>
       </c>
       <c r="D37">
         <v>7</v>
@@ -2470,21 +2455,21 @@
         <v>1.5512999999999999</v>
       </c>
       <c r="F37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G37" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D38">
         <v>8</v>
@@ -2493,21 +2478,21 @@
         <v>1000</v>
       </c>
       <c r="F38" t="s">
+        <v>75</v>
+      </c>
+      <c r="G38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
         <v>77</v>
-      </c>
-      <c r="G38" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" t="s">
-        <v>94</v>
-      </c>
-      <c r="C39" t="s">
-        <v>79</v>
       </c>
       <c r="D39">
         <v>9</v>
@@ -2516,21 +2501,21 @@
         <v>1000</v>
       </c>
       <c r="F39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" t="s">
-        <v>94</v>
-      </c>
-      <c r="C40" t="s">
-        <v>80</v>
       </c>
       <c r="D40">
         <v>10</v>
@@ -2539,21 +2524,21 @@
         <v>0.27</v>
       </c>
       <c r="F40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D41">
         <v>11</v>
@@ -2562,21 +2547,21 @@
         <v>0.95</v>
       </c>
       <c r="F41" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D42">
         <v>12</v>
@@ -2585,21 +2570,21 @@
         <v>0.9</v>
       </c>
       <c r="F42" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D43">
         <v>13</v>
@@ -2608,21 +2593,21 @@
         <v>400</v>
       </c>
       <c r="F43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -2631,21 +2616,21 @@
         <v>72</v>
       </c>
       <c r="F44" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G44" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2654,21 +2639,21 @@
         <v>243</v>
       </c>
       <c r="F45" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G45" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -2677,21 +2662,21 @@
         <v>180</v>
       </c>
       <c r="F46" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G46" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C47" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D47">
         <v>3</v>
@@ -2700,21 +2685,21 @@
         <v>2.33</v>
       </c>
       <c r="F47" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D48">
         <v>4</v>
@@ -2723,21 +2708,21 @@
         <v>26</v>
       </c>
       <c r="F48" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" t="s">
         <v>67</v>
-      </c>
-      <c r="G48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" t="s">
-        <v>69</v>
       </c>
       <c r="D49">
         <v>5</v>
@@ -2746,21 +2731,21 @@
         <v>0.45</v>
       </c>
       <c r="F49" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D50">
         <v>6</v>
@@ -2769,21 +2754,21 @@
         <v>9.4330000000000004E-3</v>
       </c>
       <c r="F50" t="s">
+        <v>70</v>
+      </c>
+      <c r="G50" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" t="s">
         <v>72</v>
-      </c>
-      <c r="G50" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" t="s">
-        <v>74</v>
       </c>
       <c r="D51">
         <v>7</v>
@@ -2792,21 +2777,21 @@
         <v>1.5512999999999999</v>
       </c>
       <c r="F51" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G51" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D52">
         <v>8</v>
@@ -2815,21 +2800,21 @@
         <v>1000</v>
       </c>
       <c r="F52" t="s">
+        <v>75</v>
+      </c>
+      <c r="G52" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" t="s">
         <v>77</v>
-      </c>
-      <c r="G52" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" t="s">
-        <v>96</v>
-      </c>
-      <c r="C53" t="s">
-        <v>79</v>
       </c>
       <c r="D53">
         <v>9</v>
@@ -2838,21 +2823,21 @@
         <v>1000</v>
       </c>
       <c r="F53" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G53" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" t="s">
-        <v>96</v>
-      </c>
-      <c r="C54" t="s">
-        <v>80</v>
       </c>
       <c r="D54">
         <v>10</v>
@@ -2861,21 +2846,21 @@
         <v>0.27</v>
       </c>
       <c r="F54" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G54" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C55" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D55">
         <v>11</v>
@@ -2884,21 +2869,21 @@
         <v>0.95</v>
       </c>
       <c r="F55" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D56">
         <v>12</v>
@@ -2907,21 +2892,21 @@
         <v>0.9</v>
       </c>
       <c r="F56" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G56" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C57" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D57">
         <v>13</v>
@@ -2930,10 +2915,10 @@
         <v>400</v>
       </c>
       <c r="F57" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G57" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2945,81 +2930,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582C6D20-8276-4D8D-A540-E889EFB05E57}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="161" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="D5" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -3029,88 +3014,72 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B0404B-9994-498F-B4BE-63E960C20C4D}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="185" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
         <v>90</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C4">
+        <v>4500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>91</v>
       </c>
-      <c r="C3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4">
-        <v>4500000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5">
+      <c r="C5">
         <v>1000000</v>
       </c>
     </row>

</xml_diff>